<commit_message>
feat: numerical inputs for priority & weight
</commit_message>
<xml_diff>
--- a/app/public/client/assets/template.xlsx
+++ b/app/public/client/assets/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10467833-3725-4C7D-BEE9-C44CBE2FE3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D520E28-43D3-4158-B9AD-5DF77C45E13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E3CD1F63-FE50-4CD3-8372-3C537BE4809C}"/>
   </bookViews>
@@ -41,12 +41,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Priority (1-10)</t>
-  </si>
-  <si>
-    <t>Weight (1-10)</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
@@ -72,6 +66,12 @@
   </si>
   <si>
     <t>school.mse1500.tests</t>
+  </si>
+  <si>
+    <t>Priority (0-100)</t>
+  </si>
+  <si>
+    <t>Weight (0-100)</t>
   </si>
 </sst>
 </file>
@@ -445,14 +445,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.140625" style="1" customWidth="1"/>
     <col min="5" max="6" width="21.5703125" style="1"/>
     <col min="7" max="7" width="43.140625" style="1" customWidth="1"/>
@@ -464,36 +464,36 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="5">
         <v>45170</v>
@@ -502,21 +502,21 @@
         <v>45179</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="5">
         <v>45179</v>
@@ -525,7 +525,7 @@
         <v>45189</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: add missing template.xlsx
</commit_message>
<xml_diff>
--- a/app/public/client/assets/template.xlsx
+++ b/app/public/client/assets/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7877249-CEE5-47B0-8B93-BCB829D4A38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B11DDE4-F57A-4AB6-B298-B75E6E439021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Project</t>
   </si>
@@ -81,25 +81,6 @@
       </rPr>
       <t>(0-100)</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Earliest Date
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>(M/D/YYYY; or  RefID for parent task)</t>
-    </r>
-  </si>
-  <si>
-    <t>A</t>
   </si>
   <si>
     <r>
@@ -151,6 +132,34 @@
       </rPr>
       <t>(M/D/YYYY)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Earliest Date
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(M/D/YYYY; or comma-delimited RefIDs for depended tasks)</t>
+    </r>
+  </si>
+  <si>
+    <t>Example: HW 2</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A1,A2</t>
   </si>
 </sst>
 </file>
@@ -422,12 +431,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -437,7 +446,7 @@
     <col min="3" max="3" width="11" style="6" customWidth="1"/>
     <col min="4" max="4" width="9.26953125" style="6" customWidth="1"/>
     <col min="5" max="5" width="27.6328125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.36328125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21.81640625" style="7" customWidth="1"/>
     <col min="7" max="7" width="13.6328125" style="7" customWidth="1"/>
     <col min="8" max="8" width="14.7265625" style="7" customWidth="1"/>
     <col min="9" max="9" width="43.08984375" style="1" customWidth="1"/>
@@ -446,10 +455,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>8</v>
@@ -461,13 +470,13 @@
         <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>1</v>
@@ -475,7 +484,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -513,13 +522,39 @@
         <v>6</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="H3" s="7">
         <v>45920</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6">
+        <v>40</v>
+      </c>
+      <c r="D4" s="6">
+        <v>70</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="7">
+        <v>45919</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>